<commit_message>
load test excel modified
</commit_message>
<xml_diff>
--- a/resources/Radom_Data_User_Api_Load_Testing .xlsx
+++ b/resources/Radom_Data_User_Api_Load_Testing .xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Load Test Strategy</t>
   </si>
@@ -37,15 +37,27 @@
     <t>Error %</t>
   </si>
   <si>
+    <t>Thoughput per test</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
     <t>Test Value</t>
   </si>
   <si>
+    <t>Test Completed Successfully without any error and Loss of Throughput</t>
+  </si>
+  <si>
     <t>Expected TPS</t>
   </si>
   <si>
     <t>Test - 1</t>
   </si>
   <si>
+    <t>2.8(upto 1d.p)</t>
+  </si>
+  <si>
     <t>Test - 2</t>
   </si>
   <si>
@@ -56,13 +68,19 @@
   </si>
   <si>
     <t>Actual TPS</t>
+  </si>
+  <si>
+    <t>2.78(upto 2d.p)</t>
+  </si>
+  <si>
+    <t>Load test Successful. Actual TPS and Expected TPS remained the same.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -80,6 +98,18 @@
       <b/>
       <u/>
       <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -126,7 +156,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border/>
     <border>
       <left style="thin">
@@ -168,6 +198,36 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -176,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -197,7 +257,13 @@
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="4" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
@@ -209,13 +275,24 @@
     <xf borderId="4" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="6" fontId="1" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -433,6 +510,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="5" max="5" width="14.25"/>
+    <col customWidth="1" min="7" max="7" width="16.25"/>
+    <col customWidth="1" min="8" max="8" width="24.38"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -442,7 +524,9 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
@@ -452,7 +536,9 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="3"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
@@ -473,10 +559,16 @@
       <c r="F3" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="G3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" s="6">
         <v>12.0</v>
@@ -491,6 +583,8 @@
         <v>120000.0</v>
       </c>
       <c r="F4" s="7"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="7"/>
     </row>
     <row r="5">
       <c r="A5" s="7"/>
@@ -508,152 +602,187 @@
         <v>10000</v>
       </c>
       <c r="F5" s="7"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10">
+      <c r="A6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12">
         <v>0.0</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="12">
         <v>1.0</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="13">
         <f>E5/D5</f>
         <v>2.777777778</v>
       </c>
-      <c r="F6" s="9"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="14"/>
     </row>
     <row r="7">
-      <c r="A7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="10">
+      <c r="A7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12">
         <v>1.0</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="12">
         <v>60.0</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="11">
         <f>E6*D7</f>
         <v>166.6666667</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="15">
         <v>0.0</v>
       </c>
+      <c r="G7" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="14"/>
     </row>
     <row r="8">
-      <c r="A8" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10">
+      <c r="A8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12">
         <v>5.0</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="12">
         <f>C8*D7</f>
         <v>300</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="11">
         <f>E6*D8</f>
         <v>833.3333333</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="15">
         <v>0.0</v>
       </c>
+      <c r="G8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="14"/>
     </row>
     <row r="9">
-      <c r="A9" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10">
+      <c r="A9" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12">
         <v>10.0</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="11">
         <f>C9*D7</f>
         <v>600</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="11">
         <f>D9*E6</f>
         <v>1666.666667</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="15">
         <v>0.0</v>
       </c>
+      <c r="G9" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="14"/>
     </row>
     <row r="10">
-      <c r="A10" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10">
+      <c r="A10" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12">
         <v>15.0</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="11">
         <f>C10*D7</f>
         <v>900</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="11">
         <f>D10*E6</f>
         <v>2500</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="15">
         <v>0.0</v>
       </c>
+      <c r="G10" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="16"/>
     </row>
     <row r="11">
-      <c r="A11" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="11">
-        <f>E10/D10</f>
-        <v>2.777777778</v>
-      </c>
-      <c r="F11" s="9"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
+      <c r="A11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" ht="37.5" customHeight="1">
+      <c r="A12" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="3"/>
     </row>
     <row r="13">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="21"/>
     </row>
     <row r="14">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="21"/>
     </row>
     <row r="15">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="H5:H10"/>
+    <mergeCell ref="A12:H12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="A2"/>

</xml_diff>